<commit_message>
Add verse range filter for Psalms 119 and change chapter label to 편 for Psalms
</commit_message>
<xml_diff>
--- a/assets/Proclaim.xlsx
+++ b/assets/Proclaim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerus\StudioProjects\proclaim\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224B1A61-58E9-4257-B7B2-AED24509A00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD45324-735F-416A-AB5C-10460490BE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Testament" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6165" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6189" uniqueCount="772">
   <si>
     <t>Date</t>
   </si>
@@ -2323,6 +2323,26 @@
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>1-48</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>49-96</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>97-136</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>137-176</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verse</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2333,7 +2353,7 @@
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2376,6 +2396,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2403,7 +2430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2440,6 +2467,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2658,14 +2689,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B356" workbookViewId="0">
-      <selection activeCell="D285" sqref="D285:G367"/>
+    <sheetView topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="C363" sqref="C363"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="28" width="8.7265625" customWidth="1"/>
+    <col min="1" max="7" width="17.73046875" customWidth="1"/>
+    <col min="8" max="28" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" customHeight="1">
@@ -9392,10 +9423,10 @@
         <v>424</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>399</v>
+        <v>426</v>
       </c>
       <c r="C293" s="6" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="D293" s="6">
         <v>1</v>
@@ -9924,7 +9955,7 @@
         <v>426</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>427</v>
+        <v>454</v>
       </c>
       <c r="D316" s="6">
         <v>1</v>
@@ -9993,7 +10024,7 @@
         <v>453</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="D319" s="6">
         <v>1</v>
@@ -10537,7 +10568,7 @@
         <v>460</v>
       </c>
       <c r="C342" s="6" t="s">
-        <v>461</v>
+        <v>488</v>
       </c>
       <c r="D342" s="6">
         <v>1</v>
@@ -10675,7 +10706,7 @@
         <v>487</v>
       </c>
       <c r="C348" s="6" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="D348" s="6">
         <v>1</v>
@@ -10767,7 +10798,7 @@
         <v>497</v>
       </c>
       <c r="C352" s="6" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="D352" s="6">
         <v>1</v>
@@ -10790,7 +10821,7 @@
         <v>505</v>
       </c>
       <c r="C353" s="6" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="D353" s="6">
         <v>1</v>
@@ -10859,7 +10890,7 @@
         <v>510</v>
       </c>
       <c r="C356" s="6" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="D356" s="6">
         <v>1</v>
@@ -10882,7 +10913,7 @@
         <v>516</v>
       </c>
       <c r="C357" s="6" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="D357" s="6">
         <v>1</v>
@@ -10905,7 +10936,7 @@
         <v>521</v>
       </c>
       <c r="C358" s="6" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="D358" s="6">
         <v>1</v>
@@ -10951,7 +10982,7 @@
         <v>526</v>
       </c>
       <c r="C360" s="6" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="D360" s="6">
         <v>1</v>
@@ -10974,7 +11005,7 @@
         <v>532</v>
       </c>
       <c r="C361" s="6" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="D361" s="6">
         <v>1</v>
@@ -10997,7 +11028,7 @@
         <v>537</v>
       </c>
       <c r="C362" s="6" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="D362" s="6">
         <v>1</v>
@@ -11020,7 +11051,7 @@
         <v>542</v>
       </c>
       <c r="C363" s="6" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="D363" s="6">
         <v>1</v>
@@ -11043,7 +11074,7 @@
         <v>547</v>
       </c>
       <c r="C364" s="6" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="D364" s="6">
         <v>1</v>
@@ -11112,7 +11143,7 @@
         <v>552</v>
       </c>
       <c r="C367" s="6" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="D367" s="6">
         <v>1</v>
@@ -15585,15 +15616,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A361" workbookViewId="0">
-      <selection activeCell="C369" sqref="C369:G377"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="28" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" customWidth="1"/>
+    <col min="2" max="7" width="17.53125" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" customWidth="1"/>
+    <col min="9" max="28" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" customHeight="1">
@@ -15618,8 +15650,8 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
+      <c r="H1" s="14" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1">
@@ -16703,7 +16735,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.5" customHeight="1">
+    <row r="49" spans="1:8" ht="16.5" customHeight="1">
       <c r="A49" s="5" t="s">
         <v>63</v>
       </c>
@@ -16725,8 +16757,11 @@
       <c r="G49" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H49" s="13" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16.5" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>64</v>
       </c>
@@ -16748,8 +16783,11 @@
       <c r="G50" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H50" s="13" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="16.5" customHeight="1">
       <c r="A51" s="5" t="s">
         <v>69</v>
       </c>
@@ -16771,8 +16809,11 @@
       <c r="G51" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H51" s="13" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="16.5" customHeight="1">
       <c r="A52" s="5" t="s">
         <v>70</v>
       </c>
@@ -16794,8 +16835,11 @@
       <c r="G52" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H52" s="13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16.5" customHeight="1">
       <c r="A53" s="5" t="s">
         <v>71</v>
       </c>
@@ -16818,7 +16862,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16.5" customHeight="1">
+    <row r="54" spans="1:8" ht="16.5" customHeight="1">
       <c r="A54" s="5" t="s">
         <v>72</v>
       </c>
@@ -16841,7 +16885,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="16.5" customHeight="1">
+    <row r="55" spans="1:8" ht="16.5" customHeight="1">
       <c r="A55" s="5" t="s">
         <v>73</v>
       </c>
@@ -16864,7 +16908,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16.5" customHeight="1">
+    <row r="56" spans="1:8" ht="16.5" customHeight="1">
       <c r="A56" s="5" t="s">
         <v>74</v>
       </c>
@@ -16887,7 +16931,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.5" customHeight="1">
+    <row r="57" spans="1:8" ht="16.5" customHeight="1">
       <c r="A57" s="5" t="s">
         <v>75</v>
       </c>
@@ -16910,7 +16954,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16.5" customHeight="1">
+    <row r="58" spans="1:8" ht="16.5" customHeight="1">
       <c r="A58" s="5" t="s">
         <v>76</v>
       </c>
@@ -16933,7 +16977,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="16.5" customHeight="1">
+    <row r="59" spans="1:8" ht="16.5" customHeight="1">
       <c r="A59" s="5" t="s">
         <v>77</v>
       </c>
@@ -16956,7 +17000,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="16.5" customHeight="1">
+    <row r="60" spans="1:8" ht="16.5" customHeight="1">
       <c r="A60" s="5" t="s">
         <v>78</v>
       </c>
@@ -16979,7 +17023,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="16.5" customHeight="1">
+    <row r="61" spans="1:8" ht="16.5" customHeight="1">
       <c r="A61" s="5" t="s">
         <v>79</v>
       </c>
@@ -17002,7 +17046,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="16.5" customHeight="1">
+    <row r="62" spans="1:8" ht="16.5" customHeight="1">
       <c r="A62" s="5" t="s">
         <v>80</v>
       </c>
@@ -17025,7 +17069,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="16.5" customHeight="1">
+    <row r="63" spans="1:8" ht="16.5" customHeight="1">
       <c r="A63" s="5" t="s">
         <v>81</v>
       </c>
@@ -17048,7 +17092,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16.5" customHeight="1">
+    <row r="64" spans="1:8" ht="16.5" customHeight="1">
       <c r="A64" s="5" t="s">
         <v>82</v>
       </c>
@@ -18101,6 +18145,9 @@
       <c r="G108" s="5" t="s">
         <v>679</v>
       </c>
+      <c r="H108" s="13" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="109" spans="1:28" ht="16.5" customHeight="1">
       <c r="A109" s="5" t="s">
@@ -18124,6 +18171,9 @@
       <c r="G109" s="5" t="s">
         <v>679</v>
       </c>
+      <c r="H109" s="13" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="110" spans="1:28" ht="16.5" customHeight="1">
       <c r="A110" s="5" t="s">
@@ -18147,6 +18197,9 @@
       <c r="G110" s="5" t="s">
         <v>679</v>
       </c>
+      <c r="H110" s="13" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="111" spans="1:28" ht="16.5" customHeight="1">
       <c r="A111" s="5" t="s">
@@ -18170,6 +18223,9 @@
       <c r="G111" s="5" t="s">
         <v>679</v>
       </c>
+      <c r="H111" s="13" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="112" spans="1:28" ht="16.5" customHeight="1">
       <c r="A112" s="5" t="s">
@@ -19298,7 +19354,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="16.5" customHeight="1">
+    <row r="161" spans="1:8" ht="16.5" customHeight="1">
       <c r="A161" s="5" t="s">
         <v>227</v>
       </c>
@@ -19321,7 +19377,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="16.5" customHeight="1">
+    <row r="162" spans="1:8" ht="16.5" customHeight="1">
       <c r="A162" s="5" t="s">
         <v>229</v>
       </c>
@@ -19344,7 +19400,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="16.5" customHeight="1">
+    <row r="163" spans="1:8" ht="16.5" customHeight="1">
       <c r="A163" s="5" t="s">
         <v>231</v>
       </c>
@@ -19367,7 +19423,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="16.5" customHeight="1">
+    <row r="164" spans="1:8" ht="16.5" customHeight="1">
       <c r="A164" s="5" t="s">
         <v>233</v>
       </c>
@@ -19390,7 +19446,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="16.5" customHeight="1">
+    <row r="165" spans="1:8" ht="16.5" customHeight="1">
       <c r="A165" s="5" t="s">
         <v>235</v>
       </c>
@@ -19413,7 +19469,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="16.5" customHeight="1">
+    <row r="166" spans="1:8" ht="16.5" customHeight="1">
       <c r="A166" s="5" t="s">
         <v>237</v>
       </c>
@@ -19436,7 +19492,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="16.5" customHeight="1">
+    <row r="167" spans="1:8" ht="16.5" customHeight="1">
       <c r="A167" s="5" t="s">
         <v>239</v>
       </c>
@@ -19458,8 +19514,11 @@
       <c r="G167" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H167" s="13" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="16.5" customHeight="1">
       <c r="A168" s="5" t="s">
         <v>241</v>
       </c>
@@ -19481,8 +19540,11 @@
       <c r="G168" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H168" s="13" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="16.5" customHeight="1">
       <c r="A169" s="5" t="s">
         <v>243</v>
       </c>
@@ -19504,8 +19566,11 @@
       <c r="G169" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H169" s="13" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="16.5" customHeight="1">
       <c r="A170" s="5" t="s">
         <v>247</v>
       </c>
@@ -19527,8 +19592,11 @@
       <c r="G170" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H170" s="13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="16.5" customHeight="1">
       <c r="A171" s="5" t="s">
         <v>248</v>
       </c>
@@ -19551,7 +19619,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="16.5" customHeight="1">
+    <row r="172" spans="1:8" ht="16.5" customHeight="1">
       <c r="A172" s="5" t="s">
         <v>249</v>
       </c>
@@ -19574,7 +19642,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="16.5" customHeight="1">
+    <row r="173" spans="1:8" ht="16.5" customHeight="1">
       <c r="A173" s="5" t="s">
         <v>250</v>
       </c>
@@ -19597,7 +19665,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="16.5" customHeight="1">
+    <row r="174" spans="1:8" ht="16.5" customHeight="1">
       <c r="A174" s="5" t="s">
         <v>251</v>
       </c>
@@ -19620,7 +19688,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="16.5" customHeight="1">
+    <row r="175" spans="1:8" ht="16.5" customHeight="1">
       <c r="A175" s="5" t="s">
         <v>252</v>
       </c>
@@ -19643,7 +19711,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="16.5" customHeight="1">
+    <row r="176" spans="1:8" ht="16.5" customHeight="1">
       <c r="A176" s="5" t="s">
         <v>253</v>
       </c>
@@ -20770,7 +20838,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="16.5" customHeight="1">
+    <row r="225" spans="1:8" ht="16.5" customHeight="1">
       <c r="A225" s="5" t="s">
         <v>333</v>
       </c>
@@ -20793,7 +20861,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="16.5" customHeight="1">
+    <row r="226" spans="1:8" ht="16.5" customHeight="1">
       <c r="A226" s="5" t="s">
         <v>334</v>
       </c>
@@ -20816,7 +20884,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="16.5" customHeight="1">
+    <row r="227" spans="1:8" ht="16.5" customHeight="1">
       <c r="A227" s="5" t="s">
         <v>335</v>
       </c>
@@ -20839,7 +20907,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="16.5" customHeight="1">
+    <row r="228" spans="1:8" ht="16.5" customHeight="1">
       <c r="A228" s="5" t="s">
         <v>336</v>
       </c>
@@ -20862,7 +20930,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="16.5" customHeight="1">
+    <row r="229" spans="1:8" ht="16.5" customHeight="1">
       <c r="A229" s="5" t="s">
         <v>341</v>
       </c>
@@ -20885,7 +20953,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="16.5" customHeight="1">
+    <row r="230" spans="1:8" ht="16.5" customHeight="1">
       <c r="A230" s="5" t="s">
         <v>342</v>
       </c>
@@ -20908,7 +20976,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="16.5" customHeight="1">
+    <row r="231" spans="1:8" ht="16.5" customHeight="1">
       <c r="A231" s="5" t="s">
         <v>343</v>
       </c>
@@ -20931,7 +20999,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="16.5" customHeight="1">
+    <row r="232" spans="1:8" ht="16.5" customHeight="1">
       <c r="A232" s="5" t="s">
         <v>347</v>
       </c>
@@ -20953,8 +21021,11 @@
       <c r="G232" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H232" s="13" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="16.5" customHeight="1">
       <c r="A233" s="5" t="s">
         <v>348</v>
       </c>
@@ -20976,8 +21047,11 @@
       <c r="G233" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H233" s="13" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="16.5" customHeight="1">
       <c r="A234" s="5" t="s">
         <v>349</v>
       </c>
@@ -20999,8 +21073,11 @@
       <c r="G234" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H234" s="13" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="16.5" customHeight="1">
       <c r="A235" s="5" t="s">
         <v>350</v>
       </c>
@@ -21022,8 +21099,11 @@
       <c r="G235" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H235" s="13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="16.5" customHeight="1">
       <c r="A236" s="5" t="s">
         <v>351</v>
       </c>
@@ -21046,7 +21126,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="16.5" customHeight="1">
+    <row r="237" spans="1:8" ht="16.5" customHeight="1">
       <c r="A237" s="5" t="s">
         <v>352</v>
       </c>
@@ -21069,7 +21149,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="16.5" customHeight="1">
+    <row r="238" spans="1:8" ht="16.5" customHeight="1">
       <c r="A238" s="5" t="s">
         <v>353</v>
       </c>
@@ -21092,7 +21172,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="16.5" customHeight="1">
+    <row r="239" spans="1:8" ht="16.5" customHeight="1">
       <c r="A239" s="5" t="s">
         <v>354</v>
       </c>
@@ -21115,7 +21195,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="16.5" customHeight="1">
+    <row r="240" spans="1:8" ht="16.5" customHeight="1">
       <c r="A240" s="5" t="s">
         <v>355</v>
       </c>
@@ -22242,7 +22322,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="289" spans="1:7" ht="16.5" customHeight="1">
+    <row r="289" spans="1:8" ht="16.5" customHeight="1">
       <c r="A289" s="5" t="s">
         <v>420</v>
       </c>
@@ -22265,7 +22345,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="16.5" customHeight="1">
+    <row r="290" spans="1:8" ht="16.5" customHeight="1">
       <c r="A290" s="5" t="s">
         <v>421</v>
       </c>
@@ -22288,7 +22368,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="291" spans="1:7" ht="16.5" customHeight="1">
+    <row r="291" spans="1:8" ht="16.5" customHeight="1">
       <c r="A291" s="5" t="s">
         <v>422</v>
       </c>
@@ -22311,7 +22391,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="292" spans="1:7" ht="16.5" customHeight="1">
+    <row r="292" spans="1:8" ht="16.5" customHeight="1">
       <c r="A292" s="5" t="s">
         <v>423</v>
       </c>
@@ -22334,7 +22414,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="293" spans="1:7" ht="16.5" customHeight="1">
+    <row r="293" spans="1:8" ht="16.5" customHeight="1">
       <c r="A293" s="5" t="s">
         <v>424</v>
       </c>
@@ -22356,8 +22436,11 @@
       <c r="G293" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="294" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H293" s="13" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" ht="16.5" customHeight="1">
       <c r="A294" s="5" t="s">
         <v>425</v>
       </c>
@@ -22379,8 +22462,11 @@
       <c r="G294" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="295" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H294" s="13" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" ht="16.5" customHeight="1">
       <c r="A295" s="5" t="s">
         <v>430</v>
       </c>
@@ -22402,8 +22488,11 @@
       <c r="G295" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="296" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H295" s="13" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" ht="16.5" customHeight="1">
       <c r="A296" s="5" t="s">
         <v>431</v>
       </c>
@@ -22425,8 +22514,11 @@
       <c r="G296" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="297" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H296" s="13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" ht="16.5" customHeight="1">
       <c r="A297" s="5" t="s">
         <v>432</v>
       </c>
@@ -22449,7 +22541,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="298" spans="1:7" ht="16.5" customHeight="1">
+    <row r="298" spans="1:8" ht="16.5" customHeight="1">
       <c r="A298" s="5" t="s">
         <v>433</v>
       </c>
@@ -22472,7 +22564,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="299" spans="1:7" ht="16.5" customHeight="1">
+    <row r="299" spans="1:8" ht="16.5" customHeight="1">
       <c r="A299" s="5" t="s">
         <v>434</v>
       </c>
@@ -22495,7 +22587,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="300" spans="1:7" ht="16.5" customHeight="1">
+    <row r="300" spans="1:8" ht="16.5" customHeight="1">
       <c r="A300" s="5" t="s">
         <v>435</v>
       </c>
@@ -22518,7 +22610,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="301" spans="1:7" ht="16.5" customHeight="1">
+    <row r="301" spans="1:8" ht="16.5" customHeight="1">
       <c r="A301" s="5" t="s">
         <v>436</v>
       </c>
@@ -22541,7 +22633,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="302" spans="1:7" ht="16.5" customHeight="1">
+    <row r="302" spans="1:8" ht="16.5" customHeight="1">
       <c r="A302" s="5" t="s">
         <v>437</v>
       </c>
@@ -22564,7 +22656,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="16.5" customHeight="1">
+    <row r="303" spans="1:8" ht="16.5" customHeight="1">
       <c r="A303" s="5" t="s">
         <v>438</v>
       </c>
@@ -22587,7 +22679,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="304" spans="1:7" ht="16.5" customHeight="1">
+    <row r="304" spans="1:8" ht="16.5" customHeight="1">
       <c r="A304" s="5" t="s">
         <v>439</v>
       </c>
@@ -23346,7 +23438,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="16.5" customHeight="1">
+    <row r="337" spans="1:8" ht="16.5" customHeight="1">
       <c r="A337" s="5" t="s">
         <v>480</v>
       </c>
@@ -23369,7 +23461,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="338" spans="1:7" ht="16.5" customHeight="1">
+    <row r="338" spans="1:8" ht="16.5" customHeight="1">
       <c r="A338" s="5" t="s">
         <v>481</v>
       </c>
@@ -23392,7 +23484,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="339" spans="1:7" ht="16.5" customHeight="1">
+    <row r="339" spans="1:8" ht="16.5" customHeight="1">
       <c r="A339" s="5" t="s">
         <v>482</v>
       </c>
@@ -23415,7 +23507,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="340" spans="1:7" ht="16.5" customHeight="1">
+    <row r="340" spans="1:8" ht="16.5" customHeight="1">
       <c r="A340" s="5" t="s">
         <v>483</v>
       </c>
@@ -23438,7 +23530,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="16.5" customHeight="1">
+    <row r="341" spans="1:8" ht="16.5" customHeight="1">
       <c r="A341" s="5" t="s">
         <v>484</v>
       </c>
@@ -23461,7 +23553,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="342" spans="1:7" ht="16.5" customHeight="1">
+    <row r="342" spans="1:8" ht="16.5" customHeight="1">
       <c r="A342" s="5" t="s">
         <v>485</v>
       </c>
@@ -23484,7 +23576,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="16.5" customHeight="1">
+    <row r="343" spans="1:8" ht="16.5" customHeight="1">
       <c r="A343" s="5" t="s">
         <v>486</v>
       </c>
@@ -23507,7 +23599,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="16.5" customHeight="1">
+    <row r="344" spans="1:8" ht="16.5" customHeight="1">
       <c r="A344" s="5" t="s">
         <v>491</v>
       </c>
@@ -23530,7 +23622,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="345" spans="1:7" ht="16.5" customHeight="1">
+    <row r="345" spans="1:8" ht="16.5" customHeight="1">
       <c r="A345" s="5" t="s">
         <v>492</v>
       </c>
@@ -23553,7 +23645,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="16.5" customHeight="1">
+    <row r="346" spans="1:8" ht="16.5" customHeight="1">
       <c r="A346" s="5" t="s">
         <v>493</v>
       </c>
@@ -23576,7 +23668,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="347" spans="1:7" ht="16.5" customHeight="1">
+    <row r="347" spans="1:8" ht="16.5" customHeight="1">
       <c r="A347" s="5" t="s">
         <v>494</v>
       </c>
@@ -23599,7 +23691,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="348" spans="1:7" ht="16.5" customHeight="1">
+    <row r="348" spans="1:8" ht="16.5" customHeight="1">
       <c r="A348" s="5" t="s">
         <v>495</v>
       </c>
@@ -23622,7 +23714,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="349" spans="1:7" ht="16.5" customHeight="1">
+    <row r="349" spans="1:8" ht="16.5" customHeight="1">
       <c r="A349" s="5" t="s">
         <v>496</v>
       </c>
@@ -23645,7 +23737,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="16.5" customHeight="1">
+    <row r="350" spans="1:8" ht="16.5" customHeight="1">
       <c r="A350" s="5" t="s">
         <v>501</v>
       </c>
@@ -23668,7 +23760,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="16.5" customHeight="1">
+    <row r="351" spans="1:8" ht="16.5" customHeight="1">
       <c r="A351" s="5" t="s">
         <v>502</v>
       </c>
@@ -23691,7 +23783,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="16.5" customHeight="1">
+    <row r="352" spans="1:8" ht="16.5" customHeight="1">
       <c r="A352" s="5" t="s">
         <v>503</v>
       </c>
@@ -23713,8 +23805,11 @@
       <c r="G352" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="353" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H352" s="13" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" ht="16.5" customHeight="1">
       <c r="A353" s="5" t="s">
         <v>504</v>
       </c>
@@ -23736,8 +23831,11 @@
       <c r="G353" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="354" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H353" s="13" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" ht="16.5" customHeight="1">
       <c r="A354" s="5" t="s">
         <v>509</v>
       </c>
@@ -23759,8 +23857,11 @@
       <c r="G354" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="355" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H354" s="13" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" ht="16.5" customHeight="1">
       <c r="A355" s="5" t="s">
         <v>514</v>
       </c>
@@ -23782,8 +23883,11 @@
       <c r="G355" s="5" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="356" spans="1:7" ht="16.5" customHeight="1">
+      <c r="H355" s="13" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" ht="16.5" customHeight="1">
       <c r="A356" s="5" t="s">
         <v>515</v>
       </c>
@@ -23806,7 +23910,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="16.5" customHeight="1">
+    <row r="357" spans="1:8" ht="16.5" customHeight="1">
       <c r="A357" s="5" t="s">
         <v>515</v>
       </c>
@@ -23829,7 +23933,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="358" spans="1:7" ht="16.5" customHeight="1">
+    <row r="358" spans="1:8" ht="16.5" customHeight="1">
       <c r="A358" s="5" t="s">
         <v>520</v>
       </c>
@@ -23852,7 +23956,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="359" spans="1:7" ht="16.5" customHeight="1">
+    <row r="359" spans="1:8" ht="16.5" customHeight="1">
       <c r="A359" s="5" t="s">
         <v>525</v>
       </c>
@@ -23875,7 +23979,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="360" spans="1:7" ht="16.5" customHeight="1">
+    <row r="360" spans="1:8" ht="16.5" customHeight="1">
       <c r="A360" s="5" t="s">
         <v>530</v>
       </c>
@@ -23898,7 +24002,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="361" spans="1:7" ht="16.5" customHeight="1">
+    <row r="361" spans="1:8" ht="16.5" customHeight="1">
       <c r="A361" s="5" t="s">
         <v>531</v>
       </c>
@@ -23921,7 +24025,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="16.5" customHeight="1">
+    <row r="362" spans="1:8" ht="16.5" customHeight="1">
       <c r="A362" s="5" t="s">
         <v>536</v>
       </c>
@@ -23944,7 +24048,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="363" spans="1:7" ht="16.5" customHeight="1">
+    <row r="363" spans="1:8" ht="16.5" customHeight="1">
       <c r="A363" s="5" t="s">
         <v>541</v>
       </c>
@@ -23967,7 +24071,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="364" spans="1:7" ht="16.5" customHeight="1">
+    <row r="364" spans="1:8" ht="16.5" customHeight="1">
       <c r="A364" s="5" t="s">
         <v>546</v>
       </c>
@@ -23990,7 +24094,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="365" spans="1:7" ht="16.5" customHeight="1">
+    <row r="365" spans="1:8" ht="16.5" customHeight="1">
       <c r="A365" s="5" t="s">
         <v>551</v>
       </c>
@@ -24013,7 +24117,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="366" spans="1:7" ht="16.5" customHeight="1">
+    <row r="366" spans="1:8" ht="16.5" customHeight="1">
       <c r="A366" s="5" t="s">
         <v>556</v>
       </c>
@@ -24036,7 +24140,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="367" spans="1:7" ht="16.5" customHeight="1">
+    <row r="367" spans="1:8" ht="16.5" customHeight="1">
       <c r="A367" s="5" t="s">
         <v>557</v>
       </c>
@@ -24059,7 +24163,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="368" spans="1:7" ht="16.5" customHeight="1">
+    <row r="368" spans="1:8" ht="16.5" customHeight="1">
       <c r="A368" s="5" t="s">
         <v>558</v>
       </c>
@@ -25047,15 +25151,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+    <sheetView topLeftCell="A351" workbookViewId="0">
       <selection activeCell="E292" sqref="E292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="7" width="17.54296875" customWidth="1"/>
-    <col min="8" max="28" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" customWidth="1"/>
+    <col min="2" max="7" width="17.53125" customWidth="1"/>
+    <col min="8" max="28" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" customHeight="1">

</xml_diff>